<commit_message>
quick fix review stars l2
</commit_message>
<xml_diff>
--- a/transformations/stimuli_l2.xlsx
+++ b/transformations/stimuli_l2.xlsx
@@ -12,30 +12,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="I1">
-      <text>
-        <t xml:space="preserve">vygenerovat, doktoři budou mít buď okolo 3, pokud se vyskytuje "mid+mid", okolo 4, pokud "mid-high" a okolo 5, pokud "high-high"
-	-Jiří Čeněk</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D1">
-      <text>
-        <t xml:space="preserve">3* nebo 5, distraktory 4
-	-Jiří Čeněk</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="143">
   <si>
     <t>nr</t>
   </si>
@@ -89,6 +67,9 @@
   </si>
   <si>
     <t>MUDr. Marie Krejčí</t>
+  </si>
+  <si>
+    <t>4.2</t>
   </si>
   <si>
     <t>b</t>
@@ -467,9 +448,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d.m"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -558,7 +536,7 @@
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -884,8 +862,8 @@
       <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8">
-        <v>45326.0</v>
+      <c r="I2" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J2" s="1">
         <v>12.0</v>
@@ -896,7 +874,7 @@
         <v>0.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -905,19 +883,19 @@
         <v>4.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="8">
-        <v>45326.0</v>
+      <c r="I3" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J3" s="1">
         <v>12.0</v>
@@ -928,7 +906,7 @@
         <v>0.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -937,19 +915,19 @@
         <v>4.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="8">
-        <v>45326.0</v>
+      <c r="I4" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J4" s="1">
         <v>12.0</v>
@@ -963,25 +941,25 @@
         <v>12</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="10">
         <v>3.0</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="8">
-        <v>45326.0</v>
+        <v>29</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J5" s="9">
         <v>57.0</v>
@@ -1010,28 +988,28 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="10">
         <v>5.0</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="8">
-        <v>45326.0</v>
+        <v>29</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J6" s="9">
         <v>57.0</v>
@@ -1060,7 +1038,7 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>13</v>
@@ -1069,19 +1047,19 @@
         <v>4.0</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="8">
-        <v>45326.0</v>
+        <v>29</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J7" s="9">
         <v>57.0</v>
@@ -1113,25 +1091,25 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3">
         <v>5.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="8">
-        <v>45326.0</v>
+        <v>38</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J8" s="1">
         <v>52.0</v>
@@ -1142,28 +1120,28 @@
         <v>2.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="3">
         <v>3.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="8">
-        <v>45326.0</v>
+        <v>38</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J9" s="1">
         <v>52.0</v>
@@ -1174,7 +1152,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -1183,19 +1161,19 @@
         <v>4.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="8">
-        <v>45326.0</v>
+        <v>38</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J10" s="1">
         <v>52.0</v>
@@ -1209,25 +1187,25 @@
         <v>12</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="10">
         <v>3.0</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="8">
-        <v>45326.0</v>
+        <v>46</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J11" s="9">
         <v>58.0</v>
@@ -1256,28 +1234,28 @@
         <v>3.0</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="10">
         <v>3.0</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="8">
-        <v>45326.0</v>
+      <c r="I12" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J12" s="9">
         <v>58.0</v>
@@ -1306,7 +1284,7 @@
         <v>3.0</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>13</v>
@@ -1315,19 +1293,19 @@
         <v>4.0</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="8">
-        <v>45326.0</v>
+        <v>46</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J13" s="9">
         <v>58.0</v>
@@ -1359,25 +1337,25 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3">
         <v>5.0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="8">
-        <v>45326.0</v>
+        <v>54</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J14" s="1">
         <v>62.0</v>
@@ -1388,28 +1366,28 @@
         <v>4.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" s="3">
         <v>5.0</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="8">
-        <v>45326.0</v>
+      <c r="I15" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J15" s="1">
         <v>62.0</v>
@@ -1420,7 +1398,7 @@
         <v>4.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1429,19 +1407,19 @@
         <v>4.0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="8">
-        <v>45326.0</v>
+        <v>54</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J16" s="1">
         <v>62.0</v>
@@ -1455,25 +1433,25 @@
         <v>12</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="10">
         <v>3.0</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="8">
-        <v>45326.0</v>
+        <v>61</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J17" s="9">
         <v>7.0</v>
@@ -1502,28 +1480,28 @@
         <v>5.0</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="10">
         <v>5.0</v>
       </c>
       <c r="E18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" s="8">
-        <v>45326.0</v>
+      <c r="I18" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J18" s="9">
         <v>7.0</v>
@@ -1552,7 +1530,7 @@
         <v>5.0</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>13</v>
@@ -1561,19 +1539,19 @@
         <v>4.0</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="8">
-        <v>45326.0</v>
+        <v>61</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J19" s="9">
         <v>7.0</v>
@@ -1605,25 +1583,25 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" s="3">
         <v>5.0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" s="8">
-        <v>45326.0</v>
+        <v>68</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J20" s="1">
         <v>61.0</v>
@@ -1634,28 +1612,28 @@
         <v>6.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D21" s="3">
         <v>3.0</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" s="8">
-        <v>45326.0</v>
+      <c r="I21" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J21" s="1">
         <v>61.0</v>
@@ -1666,7 +1644,7 @@
         <v>6.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -1675,19 +1653,19 @@
         <v>4.0</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="8">
-        <v>45326.0</v>
+        <v>68</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J22" s="1">
         <v>61.0</v>
@@ -1701,25 +1679,25 @@
         <v>12</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" s="10">
         <v>3.0</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" s="8">
-        <v>45326.0</v>
+        <v>75</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J23" s="9">
         <v>6.0</v>
@@ -1748,28 +1726,28 @@
         <v>7.0</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D24" s="10">
         <v>3.0</v>
       </c>
       <c r="E24" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" s="8">
-        <v>45326.0</v>
+      <c r="I24" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J24" s="9">
         <v>6.0</v>
@@ -1798,7 +1776,7 @@
         <v>7.0</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>13</v>
@@ -1807,19 +1785,19 @@
         <v>4.0</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="8">
-        <v>45326.0</v>
+        <v>75</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J25" s="9">
         <v>6.0</v>
@@ -1851,25 +1829,25 @@
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" s="3">
         <v>5.0</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" s="8">
-        <v>45326.0</v>
+        <v>82</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J26" s="1">
         <v>65.0</v>
@@ -1880,28 +1858,28 @@
         <v>8.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3">
         <v>5.0</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I27" s="8">
-        <v>45326.0</v>
+      <c r="I27" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J27" s="1">
         <v>65.0</v>
@@ -1912,7 +1890,7 @@
         <v>8.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>
@@ -1921,19 +1899,19 @@
         <v>4.0</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I28" s="8">
-        <v>45326.0</v>
+        <v>82</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J28" s="1">
         <v>65.0</v>
@@ -1947,25 +1925,25 @@
         <v>12</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D29" s="10">
         <v>3.0</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="8">
-        <v>45326.0</v>
+        <v>89</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J29" s="9">
         <v>69.0</v>
@@ -1994,28 +1972,28 @@
         <v>9.0</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D30" s="10">
         <v>5.0</v>
       </c>
       <c r="E30" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H30" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I30" s="8">
-        <v>45326.0</v>
+      <c r="I30" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J30" s="9">
         <v>69.0</v>
@@ -2044,7 +2022,7 @@
         <v>9.0</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
@@ -2053,19 +2031,19 @@
         <v>4.0</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I31" s="8">
-        <v>45326.0</v>
+        <v>89</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J31" s="9">
         <v>69.0</v>
@@ -2097,25 +2075,25 @@
         <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D32" s="3">
         <v>5.0</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I32" s="8">
-        <v>45326.0</v>
+        <v>96</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J32" s="1">
         <v>8.0</v>
@@ -2126,28 +2104,28 @@
         <v>10.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D33" s="3">
         <v>3.0</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H33" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I33" s="8">
-        <v>45326.0</v>
+      <c r="I33" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J33" s="1">
         <v>8.0</v>
@@ -2158,7 +2136,7 @@
         <v>10.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>13</v>
@@ -2167,19 +2145,19 @@
         <v>4.0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I34" s="8">
-        <v>45326.0</v>
+        <v>96</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J34" s="1">
         <v>8.0</v>
@@ -2193,25 +2171,25 @@
         <v>12</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D35" s="10">
         <v>3.0</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="I35" s="8">
-        <v>45326.0</v>
+        <v>103</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J35" s="9">
         <v>54.0</v>
@@ -2240,28 +2218,28 @@
         <v>11.0</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D36" s="10">
         <v>3.0</v>
       </c>
       <c r="E36" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H36" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="F36" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="I36" s="8">
-        <v>45326.0</v>
+      <c r="I36" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J36" s="9">
         <v>54.0</v>
@@ -2290,7 +2268,7 @@
         <v>11.0</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>13</v>
@@ -2299,19 +2277,19 @@
         <v>4.0</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="I37" s="8">
-        <v>45326.0</v>
+        <v>103</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J37" s="9">
         <v>54.0</v>
@@ -2343,25 +2321,25 @@
         <v>12</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D38" s="3">
         <v>5.0</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I38" s="8">
-        <v>45326.0</v>
+        <v>110</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J38" s="1">
         <v>9.0</v>
@@ -2372,28 +2350,28 @@
         <v>12.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D39" s="3">
         <v>5.0</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I39" s="8">
-        <v>45326.0</v>
+      <c r="I39" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J39" s="1">
         <v>9.0</v>
@@ -2404,7 +2382,7 @@
         <v>12.0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -2413,19 +2391,19 @@
         <v>4.0</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I40" s="8">
-        <v>45326.0</v>
+        <v>110</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J40" s="1">
         <v>9.0</v>
@@ -2439,25 +2417,25 @@
         <v>12</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D41" s="10">
         <v>3.0</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I41" s="8">
-        <v>45326.0</v>
+        <v>117</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J41" s="9">
         <v>6.0</v>
@@ -2486,28 +2464,28 @@
         <v>13.0</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D42" s="10">
         <v>5.0</v>
       </c>
       <c r="E42" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H42" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" s="8">
-        <v>45326.0</v>
+      <c r="I42" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J42" s="9">
         <v>6.0</v>
@@ -2536,7 +2514,7 @@
         <v>13.0</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>13</v>
@@ -2545,19 +2523,19 @@
         <v>4.0</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I43" s="8">
-        <v>45326.0</v>
+        <v>117</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J43" s="9">
         <v>6.0</v>
@@ -2589,25 +2567,25 @@
         <v>12</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D44" s="3">
         <v>5.0</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I44" s="8">
-        <v>45326.0</v>
+        <v>124</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J44" s="1">
         <v>5.0</v>
@@ -2618,28 +2596,28 @@
         <v>14.0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D45" s="3">
         <v>3.0</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I45" s="8">
-        <v>45326.0</v>
+      <c r="I45" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J45" s="1">
         <v>5.0</v>
@@ -2650,7 +2628,7 @@
         <v>14.0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>13</v>
@@ -2659,19 +2637,19 @@
         <v>4.0</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I46" s="8">
-        <v>45326.0</v>
+        <v>124</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J46" s="1">
         <v>5.0</v>
@@ -2685,25 +2663,25 @@
         <v>12</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D47" s="10">
         <v>3.0</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="I47" s="8">
-        <v>45326.0</v>
+        <v>131</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J47" s="9">
         <v>8.0</v>
@@ -2732,28 +2710,28 @@
         <v>15.0</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D48" s="10">
         <v>3.0</v>
       </c>
       <c r="E48" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="F48" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="I48" s="8">
-        <v>45326.0</v>
+      <c r="I48" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J48" s="9">
         <v>8.0</v>
@@ -2782,7 +2760,7 @@
         <v>15.0</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>13</v>
@@ -2791,19 +2769,19 @@
         <v>4.0</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="I49" s="8">
-        <v>45326.0</v>
+        <v>131</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J49" s="9">
         <v>8.0</v>
@@ -2835,25 +2813,25 @@
         <v>12</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D50" s="3">
         <v>5.0</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="I50" s="8">
-        <v>45326.0</v>
+        <v>138</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J50" s="1">
         <v>8.0</v>
@@ -2864,28 +2842,28 @@
         <v>16.0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D51" s="3">
         <v>5.0</v>
       </c>
       <c r="E51" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H51" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="I51" s="8">
-        <v>45326.0</v>
+      <c r="I51" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J51" s="1">
         <v>8.0</v>
@@ -2896,7 +2874,7 @@
         <v>16.0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>13</v>
@@ -2905,19 +2883,19 @@
         <v>4.0</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="I52" s="8">
-        <v>45326.0</v>
+        <v>138</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J52" s="1">
         <v>8.0</v>
@@ -8553,7 +8531,6 @@
     </row>
   </sheetData>
   <autoFilter ref="$C$1:$C$990"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>